<commit_message>
papers and update databses
</commit_message>
<xml_diff>
--- a/markdown_gen/publications.xlsx
+++ b/markdown_gen/publications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/ht-timchen-beautiful/markdown_gen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A86DF37-EC24-DB41-B5FA-F3D747863F11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA7DEC8-E5F7-4B4E-87BC-920FA46F9165}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17980" yWindow="1240" windowWidth="26920" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="92">
   <si>
     <t>YEAR</t>
   </si>
@@ -245,6 +245,57 @@
   </si>
   <si>
     <t>ACM SIGGRPAH VRCAI</t>
+  </si>
+  <si>
+    <t>2011_SIG_revision.pdf</t>
+  </si>
+  <si>
+    <t>2013_PG_Splattering.pdf</t>
+  </si>
+  <si>
+    <t>2013_VRST_Faceton.pdf</t>
+  </si>
+  <si>
+    <t>2014_CHI_viewpoint.pdf</t>
+  </si>
+  <si>
+    <t>2014_SA_Autocomplete.pdf</t>
+  </si>
+  <si>
+    <t>2015_CHI_platener.pdf</t>
+  </si>
+  <si>
+    <t>2015_UIST_Protopiper.pdf</t>
+  </si>
+  <si>
+    <t>2016_I3D_history.pdf</t>
+  </si>
+  <si>
+    <t>2015_UIST_LaserStacker.pdf</t>
+  </si>
+  <si>
+    <t>2016_PG_icon.pdf</t>
+  </si>
+  <si>
+    <t>2016_UIST_Metamaterial.pdf</t>
+  </si>
+  <si>
+    <t>2017_CHI_TrussFab.pdf</t>
+  </si>
+  <si>
+    <t>2018_ACCESS_PredictionError.pdf</t>
+  </si>
+  <si>
+    <t>2019_CHI_HapticImmersion.pdf</t>
+  </si>
+  <si>
+    <t>2019_VRCAI_sickness.pdf</t>
+  </si>
+  <si>
+    <t>2019_TVCG_VR Fall.pdf</t>
+  </si>
+  <si>
+    <t>2020_TCDS_conflict.pdf</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1156,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1172,6 +1223,9 @@
       <c r="E3" t="s">
         <v>56</v>
       </c>
+      <c r="F3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -1189,6 +1243,9 @@
       <c r="E4" t="s">
         <v>57</v>
       </c>
+      <c r="F4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -1206,6 +1263,9 @@
       <c r="E5" t="s">
         <v>58</v>
       </c>
+      <c r="F5" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -1223,6 +1283,9 @@
       <c r="E6" t="s">
         <v>59</v>
       </c>
+      <c r="F6" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -1240,6 +1303,9 @@
       <c r="E7" t="s">
         <v>60</v>
       </c>
+      <c r="F7" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -1257,6 +1323,9 @@
       <c r="E8" t="s">
         <v>61</v>
       </c>
+      <c r="F8" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -1274,6 +1343,9 @@
       <c r="E9" t="s">
         <v>62</v>
       </c>
+      <c r="F9" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -1291,6 +1363,9 @@
       <c r="E10" t="s">
         <v>63</v>
       </c>
+      <c r="F10" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -1308,6 +1383,9 @@
       <c r="E11" t="s">
         <v>64</v>
       </c>
+      <c r="F11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -1325,6 +1403,9 @@
       <c r="E12" t="s">
         <v>66</v>
       </c>
+      <c r="F12" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1342,6 +1423,9 @@
       <c r="E13" t="s">
         <v>65</v>
       </c>
+      <c r="F13" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -1359,6 +1443,9 @@
       <c r="E14" t="s">
         <v>67</v>
       </c>
+      <c r="F14" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -1376,6 +1463,9 @@
       <c r="E15" t="s">
         <v>68</v>
       </c>
+      <c r="F15" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -1393,8 +1483,11 @@
       <c r="E16" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2013</v>
       </c>
@@ -1410,8 +1503,11 @@
       <c r="E17" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2013</v>
       </c>
@@ -1427,8 +1523,11 @@
       <c r="E18" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2011</v>
       </c>
@@ -1443,6 +1542,9 @@
       </c>
       <c r="E19" t="s">
         <v>72</v>
+      </c>
+      <c r="F19" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CHI and CVPR update
</commit_message>
<xml_diff>
--- a/markdown_gen/publications.xlsx
+++ b/markdown_gen/publications.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/GitHub/ht-timchen.github.io/markdown_gen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3BC0A1-8D6A-1A4D-96A7-B469B3D3DD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9DE842-D0F8-FD4E-BBA6-997999F44A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4180" yWindow="1820" windowWidth="27800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publications" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="176">
   <si>
     <t>YEAR</t>
   </si>
@@ -536,6 +549,30 @@
   </si>
   <si>
     <t>2024_ISBI_TVUS.pdf</t>
+  </si>
+  <si>
+    <t>CLOC: Contrastive Learning for Ordinal Classification with Multi-Margin N-pair Loss</t>
+  </si>
+  <si>
+    <t>Dileepa Pitawela, Gustavo Carneiro, Tim Chen</t>
+  </si>
+  <si>
+    <t>CVPR</t>
+  </si>
+  <si>
+    <t>2025_CVPR_Ordinal.png</t>
+  </si>
+  <si>
+    <t>2025_CHI_fatigue.pdf</t>
+  </si>
+  <si>
+    <t>2025_CHI_XRAuthor.pdf</t>
+  </si>
+  <si>
+    <t>https://youtu.be/aXunoZZKcs4</t>
+  </si>
+  <si>
+    <t>https://youtu.be/PnblYeE9gbs</t>
   </si>
 </sst>
 </file>
@@ -1426,10 +1463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1465,121 +1502,127 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2025</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="E2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2025</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>161</v>
       </c>
       <c r="E3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2025</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2024</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E4" t="s">
-        <v>147</v>
-      </c>
       <c r="F4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+      <c r="G4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2024</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>149</v>
+      <c r="B5" s="4" t="s">
+        <v>166</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>146</v>
       </c>
       <c r="E5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2024</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2024</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>158</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>2023</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E7" t="s">
-        <v>138</v>
-      </c>
-      <c r="F7" t="s">
-        <v>139</v>
-      </c>
-      <c r="G7" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1587,42 +1630,45 @@
         <v>2023</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="E8" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="F8" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="G8" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="E9" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="F9" t="s">
-        <v>145</v>
+        <v>131</v>
+      </c>
+      <c r="G9" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1630,42 +1676,39 @@
         <v>2022</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>125</v>
+        <v>141</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="E10" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="F10" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
       <c r="E11" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="F11" t="s">
-        <v>121</v>
-      </c>
-      <c r="G11" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1673,68 +1716,68 @@
         <v>2021</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>115</v>
+        <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="F12" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="G12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2021</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2021</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>99</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>98</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>2020</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" t="s">
-        <v>97</v>
-      </c>
-      <c r="G14" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1742,42 +1785,42 @@
         <v>2020</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
+        <v>97</v>
+      </c>
+      <c r="G15" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1785,131 +1828,131 @@
         <v>2019</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" t="s">
-        <v>63</v>
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="G17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2019</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2019</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>16</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>48</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="20" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>2018</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>17</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>49</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>76</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="21" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>2017</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>20</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>50</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F21" t="s">
         <v>75</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>2016</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" t="s">
-        <v>51</v>
-      </c>
-      <c r="F21" t="s">
-        <v>74</v>
-      </c>
-      <c r="G21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2016</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1917,160 +1960,160 @@
         <v>2016</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D24" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="E24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G24" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2015</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D25" t="s">
         <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2015</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2015</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>20</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>56</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" t="s">
         <v>69</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G27" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>2014</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" t="s">
-        <v>57</v>
-      </c>
-      <c r="F27" t="s">
-        <v>68</v>
-      </c>
-      <c r="G27" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2014</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2014</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>20</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>58</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" t="s">
         <v>67</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G29" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>2013</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29" t="s">
-        <v>66</v>
-      </c>
-      <c r="G29" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -2078,44 +2121,67 @@
         <v>2013</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2013</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>37</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>60</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F31" t="s">
         <v>65</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G31" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31">
+    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32">
         <v>2011</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>38</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" t="s">
         <v>61</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F32" t="s">
         <v>64</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G32" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update tag filtering: clear all tags when clicking a tag, deselect if already selected
</commit_message>
<xml_diff>
--- a/markdown_gen/publications.xlsx
+++ b/markdown_gen/publications.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1227750/GitHub/ht-timchen.github.io/markdown_gen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9C2E43-71B1-5543-8FC0-409612D4A069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C569B317-B15C-374B-AE1B-77B9B77B6D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="4360" windowWidth="31220" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30500" yWindow="6620" windowWidth="31220" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publications" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="228">
   <si>
     <t>YEAR</t>
   </si>
@@ -660,6 +660,75 @@
   </si>
   <si>
     <t>Tim Chen, Yuan Zhang, Gustavo Carneiro, Rajvinder Singh</t>
+  </si>
+  <si>
+    <t>Understanding Annotation Error Propagation and Learning an Adaptive Policy for Expert Intervention in Barrett's Video Segmentation</t>
+  </si>
+  <si>
+    <t>Lokesha Rasanjalee, Dileepa Pitawela, Jin Tan, Rajvinder Singh, Tim Chen</t>
+  </si>
+  <si>
+    <t>International Symposium on Biomedical Imaging (ISBI)</t>
+  </si>
+  <si>
+    <t>OUGS: Active View Selection via Object-aware Uncertainty Estimation in 3DGS</t>
+  </si>
+  <si>
+    <t>Haiyi Li , Qi Chen , Denis Kalkofe ,Tim Chen</t>
+  </si>
+  <si>
+    <t>Eurographics</t>
+  </si>
+  <si>
+    <t>Graphics,XR</t>
+  </si>
+  <si>
+    <t>2026_EG_OUGS.jpg</t>
+  </si>
+  <si>
+    <t>2026_ISBI_L2D.jpg</t>
+  </si>
+  <si>
+    <t>2026_ISBI_L2D.pdf</t>
+  </si>
+  <si>
+    <t>Carlos Tirado Cortes, Yiheng Chi, Juno Kim, Tim Chen</t>
+  </si>
+  <si>
+    <t>Transaction on Visualisation and Computer Graphics (IEEE VR)</t>
+  </si>
+  <si>
+    <t>2026_TVCG_Cybersickness.jpg</t>
+  </si>
+  <si>
+    <t>2026_TVCG_Cybersickness.pdf</t>
+  </si>
+  <si>
+    <t>Kinematic Sickness: Understanding Cybersickness Through Body Kinematics</t>
+  </si>
+  <si>
+    <t>L2CU: Learning to Complement Unseen Users</t>
+  </si>
+  <si>
+    <t>2025_Access_L2CU.jpg</t>
+  </si>
+  <si>
+    <t>2025_Access_L2CU.pdf</t>
+  </si>
+  <si>
+    <t>Learning To Defer To A Population With Limited Demonstrations</t>
+  </si>
+  <si>
+    <t>DICTA</t>
+  </si>
+  <si>
+    <t>2025_DICTA_L2D.jpg</t>
+  </si>
+  <si>
+    <t>2025_DICTA_L2D.pdf</t>
+  </si>
+  <si>
+    <t>Nilesh Ramgolam, Gustavo Carneiro, Tim Chen</t>
   </si>
 </sst>
 </file>
@@ -1541,10 +1610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1584,76 +1653,67 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>168</v>
+        <v>205</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>169</v>
+        <v>206</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="E2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="H2" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F2" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>159</v>
+        <v>208</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>160</v>
+        <v>209</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>161</v>
+        <v>210</v>
       </c>
       <c r="E3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="H3" t="s">
-        <v>179</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>164</v>
+        <v>219</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>165</v>
+        <v>215</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="E4" t="s">
-        <v>163</v>
+        <v>217</v>
       </c>
       <c r="F4" t="s">
-        <v>173</v>
-      </c>
-      <c r="G4" t="s">
-        <v>175</v>
+        <v>218</v>
       </c>
       <c r="H4" t="s">
         <v>179</v>
@@ -1661,137 +1721,143 @@
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2025</v>
-      </c>
-      <c r="B5" t="s">
-        <v>200</v>
-      </c>
-      <c r="C5" t="s">
-        <v>204</v>
+        <v>2026</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>203</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="F5" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="H5" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2025</v>
       </c>
-      <c r="B6" t="s">
-        <v>192</v>
-      </c>
-      <c r="C6" t="s">
-        <v>193</v>
+      <c r="B6" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>227</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>191</v>
+        <v>224</v>
       </c>
       <c r="E6" t="s">
-        <v>195</v>
+        <v>225</v>
       </c>
       <c r="F6" t="s">
-        <v>194</v>
+        <v>226</v>
       </c>
       <c r="H6" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2025</v>
       </c>
-      <c r="B7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C7" t="s">
-        <v>199</v>
+      <c r="B7" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="E7" t="s">
-        <v>196</v>
-      </c>
-      <c r="F7" t="s">
-        <v>197</v>
-      </c>
-      <c r="H7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2024</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>166</v>
+        <v>2025</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="F8" t="s">
-        <v>153</v>
+        <v>172</v>
+      </c>
+      <c r="G8" t="s">
+        <v>174</v>
       </c>
       <c r="H8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="E9" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="F9" t="s">
-        <v>154</v>
+        <v>173</v>
+      </c>
+      <c r="G9" t="s">
+        <v>175</v>
       </c>
       <c r="H9" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2024</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>156</v>
+        <v>2025</v>
+      </c>
+      <c r="B10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C10" t="s">
+        <v>204</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>157</v>
+        <v>203</v>
       </c>
       <c r="E10" t="s">
-        <v>158</v>
+        <v>201</v>
       </c>
       <c r="F10" t="s">
-        <v>167</v>
+        <v>202</v>
       </c>
       <c r="H10" t="s">
         <v>178</v>
@@ -1799,273 +1865,261 @@
     </row>
     <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
+        <v>2025</v>
+      </c>
+      <c r="B11" t="s">
+        <v>192</v>
+      </c>
+      <c r="C11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F11" t="s">
+        <v>194</v>
+      </c>
+      <c r="H11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2025</v>
+      </c>
+      <c r="B12" t="s">
+        <v>198</v>
+      </c>
+      <c r="C12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E12" t="s">
+        <v>196</v>
+      </c>
+      <c r="F12" t="s">
+        <v>197</v>
+      </c>
+      <c r="H12" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>2024</v>
       </c>
-      <c r="B11" t="s">
-        <v>186</v>
-      </c>
-      <c r="C11" t="s">
-        <v>187</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E11" t="s">
-        <v>189</v>
-      </c>
-      <c r="F11" t="s">
-        <v>190</v>
-      </c>
-      <c r="H11" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>2023</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E12" t="s">
-        <v>138</v>
-      </c>
-      <c r="F12" t="s">
-        <v>139</v>
-      </c>
-      <c r="G12" t="s">
-        <v>140</v>
-      </c>
-      <c r="H12" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>2023</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>133</v>
+      <c r="B13" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="E13" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="F13" t="s">
-        <v>131</v>
-      </c>
-      <c r="G13" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="H13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>142</v>
+        <v>149</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E14" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="F14" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="H14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2024</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" t="s">
+        <v>167</v>
+      </c>
+      <c r="H15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>2022</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E15" t="s">
-        <v>127</v>
-      </c>
-      <c r="F15" t="s">
-        <v>130</v>
-      </c>
-      <c r="H15" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>2021</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>120</v>
+        <v>2024</v>
+      </c>
+      <c r="B16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C16" t="s">
+        <v>187</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>13</v>
+        <v>188</v>
       </c>
       <c r="E16" t="s">
-        <v>122</v>
+        <v>189</v>
       </c>
       <c r="F16" t="s">
-        <v>121</v>
-      </c>
-      <c r="G16" t="s">
-        <v>123</v>
+        <v>190</v>
       </c>
       <c r="H16" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="E17" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="F17" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="G17" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="H17" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="33" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>151</v>
+        <v>132</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="E18" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="F18" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="G18" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="H18" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>7</v>
+        <v>141</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="E19" t="s">
-        <v>62</v>
+        <v>144</v>
       </c>
       <c r="F19" t="s">
-        <v>97</v>
-      </c>
-      <c r="G19" t="s">
-        <v>96</v>
+        <v>145</v>
       </c>
       <c r="H19" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>9</v>
+        <v>124</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>10</v>
+        <v>125</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>8</v>
+        <v>126</v>
       </c>
       <c r="E20" t="s">
-        <v>45</v>
+        <v>127</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="H20" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>11</v>
+        <v>119</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>46</v>
+        <v>122</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="G21" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="H21" t="s">
         <v>179</v>
@@ -2073,305 +2127,302 @@
     </row>
     <row r="22" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" t="s">
-        <v>63</v>
+        <v>113</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="E22" t="s">
-        <v>47</v>
+        <v>117</v>
       </c>
       <c r="F22" t="s">
-        <v>78</v>
+        <v>116</v>
+      </c>
+      <c r="G22" t="s">
+        <v>118</v>
       </c>
       <c r="H22" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="33" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" t="s">
-        <v>16</v>
+        <v>101</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="F23" t="s">
-        <v>77</v>
+        <v>98</v>
+      </c>
+      <c r="G23" t="s">
+        <v>102</v>
       </c>
       <c r="H23" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D24" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="F24" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="G24" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="H24" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" t="s">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F25" t="s">
-        <v>75</v>
-      </c>
-      <c r="G25" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H25" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F26" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="G26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H26" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" t="s">
+        <v>63</v>
       </c>
       <c r="E27" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F27" t="s">
-        <v>73</v>
-      </c>
-      <c r="G27" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H27" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" t="s">
+        <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F28" t="s">
-        <v>71</v>
-      </c>
-      <c r="G28" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="H28" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F29" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="G29" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H29" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E30" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F30" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G30" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H30" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D31" t="s">
-        <v>20</v>
+        <v>108</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F31" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="G31" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H31" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>2014</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>30</v>
+        <v>2016</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D32" t="s">
-        <v>31</v>
+        <v>41</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="E32" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F32" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G32" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H32" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>2014</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>32</v>
+        <v>2016</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D33" t="s">
-        <v>20</v>
+        <v>42</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="E33" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F33" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="G33" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H33" t="s">
         <v>185</v>
@@ -2379,79 +2430,209 @@
     </row>
     <row r="34" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A34">
+        <v>2015</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" t="s">
+        <v>72</v>
+      </c>
+      <c r="G34" t="s">
+        <v>88</v>
+      </c>
+      <c r="H34" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2015</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" t="s">
+        <v>70</v>
+      </c>
+      <c r="G35" t="s">
+        <v>89</v>
+      </c>
+      <c r="H35" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2015</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36" t="s">
+        <v>69</v>
+      </c>
+      <c r="G36" t="s">
+        <v>90</v>
+      </c>
+      <c r="H36" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2014</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G37" t="s">
+        <v>91</v>
+      </c>
+      <c r="H37" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2014</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" t="s">
+        <v>67</v>
+      </c>
+      <c r="G38" t="s">
+        <v>92</v>
+      </c>
+      <c r="H38" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A39">
         <v>2013</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E39" t="s">
         <v>59</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F39" t="s">
         <v>66</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G39" t="s">
         <v>93</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H39" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A35">
+    <row r="40" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A40">
         <v>2013</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D40" t="s">
         <v>37</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E40" t="s">
         <v>60</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F40" t="s">
         <v>65</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G40" t="s">
         <v>94</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H40" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36">
+    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41">
         <v>2011</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D41" t="s">
         <v>38</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E41" t="s">
         <v>61</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F41" t="s">
         <v>64</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G41" t="s">
         <v>95</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H41" t="s">
         <v>185</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Regenerate publications page and add new publication PDF
</commit_message>
<xml_diff>
--- a/markdown_gen/publications.xlsx
+++ b/markdown_gen/publications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1227750/GitHub/ht-timchen.github.io/markdown_gen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C569B317-B15C-374B-AE1B-77B9B77B6D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEE6F37-DE24-F341-97FD-EB29BB38D964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30500" yWindow="6620" windowWidth="31220" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="229">
   <si>
     <t>YEAR</t>
   </si>
@@ -729,6 +729,9 @@
   </si>
   <si>
     <t>Nilesh Ramgolam, Gustavo Carneiro, Tim Chen</t>
+  </si>
+  <si>
+    <t>2026_EG_OUGS.pdf</t>
   </si>
 </sst>
 </file>
@@ -1613,7 +1616,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1692,6 +1695,9 @@
       <c r="E3" t="s">
         <v>212</v>
       </c>
+      <c r="F3" t="s">
+        <v>228</v>
+      </c>
       <c r="H3" t="s">
         <v>211</v>
       </c>

</xml_diff>